<commit_message>
Added new users histories to the Product Backlog
</commit_message>
<xml_diff>
--- a/documentation/SCRUM Planification/Planificacion_SCRUM.xlsx
+++ b/documentation/SCRUM Planification/Planificacion_SCRUM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaulRC1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juald\OneDrive\Documentos\Juan Alberto\4º Curso\Segundo Cuatrimestre\TFG\Saluhud\documentation\SCRUM Planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08181132-0D90-453A-957C-BE971D26D7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB850C1-3EAA-4B6D-B227-6C8C52DBAACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16575" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Configuración de C3P0 dentro de Hibernate</t>
   </si>
   <si>
-    <t>Modelado en Java de las clases correspondientes a las tablas relacionadas con las recetas</t>
-  </si>
-  <si>
     <t>Modelado en la base de datos para las tablas relacionadas con el foro de la comunidad</t>
   </si>
   <si>
@@ -131,12 +128,54 @@
   <si>
     <t>Sprint 1</t>
   </si>
+  <si>
+    <t>El usuario deberá poder configurar un perfil propio, para ello se le pedirá altura, sexo, peso y edad.</t>
+  </si>
+  <si>
+    <t>El usuario podrá modificar los datos de su perfil así como llevar un seguimiento del mismo.</t>
+  </si>
+  <si>
+    <t>El usuario debería poder gestionar mediante la app cuantos vasos de agua ha tomado al día, por medio del envío de notificaciones diarias.</t>
+  </si>
+  <si>
+    <t>El usuario deberá poder configurar su periodo de sueño. Se le notificará una evaluación del mismo así como avisos para cumplir su plan de sueño.</t>
+  </si>
+  <si>
+    <t>Se deben modelar todas las tablas necesarias para el almacenamiento de todos los datos relacionados con las recetas, nombre, ingredientes, descripcion de la receta, lista de alérgenos y pasos para realizarla</t>
+  </si>
+  <si>
+    <t>Se deben modelar todas las tablas necesarias para el almacenamiento de los datos relacionados con las activididades del foro, autor, fecha del mensaje, contenido del mensaje y el hilo del mismo. En lo referente al hilo se deberá guardar, el titulo, el autor, la fecha en la que se creó y la lista de mensajes del mismo.</t>
+  </si>
+  <si>
+    <t>Se deben modelar todas las tablas necesarias para el almacenamiento de los datos relacionados con los eventos de la universidad. Se deberá recoger, una imagen del mismo si la hubiese, el nombre del evento, su descripción y la fecha del mismo.</t>
+  </si>
+  <si>
+    <t>Modelado en la base de datos de las clases correspondientes a las tablas relacionadas con las recetas</t>
+  </si>
+  <si>
+    <t>Modelado en Java de la clases correspondientes a las tablas relacionadas con las recetas</t>
+  </si>
+  <si>
+    <t>Se deben modelar las clases necesarias para el correcto funcionamiento del foro de la aplicación</t>
+  </si>
+  <si>
+    <t>Se deben modelar las clases necesarias para el correcto funcionamiento y visualización de los eventos que la universidad de huelva realice</t>
+  </si>
+  <si>
+    <t>Se deben modelar las clases necesarias para el correcto uso de los datos de los usuarios, así como para su visualización y posterior posible uso.</t>
+  </si>
+  <si>
+    <t>Se deben modelar las clases necesarias para el correcto uso de los datos relacionados con la salud de los usuarios, su visualización y uso.</t>
+  </si>
+  <si>
+    <t>Se deben modelar las clases necesarias para el correcto uso de los datos relacionados con las recetas, su visualización y uso.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +195,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -232,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -240,9 +285,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -268,6 +310,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -551,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G2140"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,251 +645,265 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>1000</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>1</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <f>SUM(D11)</f>
         <v>2.5</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
         <v>1001</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="11">
+      <c r="C11" s="12"/>
+      <c r="D11" s="10">
         <v>2.5</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
         <v>1002</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="A13" s="10">
         <v>1003</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
         <v>1004</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>1005</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
-        <v>1005</v>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13" t="s">
+        <v>35</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>1006</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
-        <v>1006</v>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13" t="s">
+        <v>36</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>1007</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
-        <v>1007</v>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="11" t="s">
+        <v>22</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>1008</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="12" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
-        <v>1008</v>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>1009</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="12" t="s">
+      <c r="B19" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
-        <v>1009</v>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="13" t="s">
+        <v>39</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>1010</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
-        <v>1010</v>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13" t="s">
+        <v>40</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>1011</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-    </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
-        <v>1011</v>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="13" t="s">
+        <v>41</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>1012</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
-        <v>1012</v>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="13" t="s">
+        <v>42</v>
       </c>
-      <c r="B22" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
         <v>1013</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="B23" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
-        <v>1014</v>
-      </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
-        <v>1015</v>
-      </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
@@ -883,11 +951,11 @@
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="A32" s="16">
         <v>2000</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>29</v>
+      <c r="B32" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -895,36 +963,52 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
+    <row r="33" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="16">
+        <v>2001</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
+    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="16">
+        <v>2002</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>33</v>
+      </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="16">
+        <v>2003</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="16">
+        <v>2004</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -19868,15 +19952,16 @@
       <c r="G2140" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4B4D1B-6AAD-4E97-A49C-7BF73E146AAB}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -19888,10 +19973,9 @@
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadida descripcion a las tareas configuracion C3P0 y creación de las clases necesarias para la conexión a la base de datos
</commit_message>
<xml_diff>
--- a/documentation/SCRUM Planification/Planificacion_SCRUM.xlsx
+++ b/documentation/SCRUM Planification/Planificacion_SCRUM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juald\OneDrive\Documentos\Juan Alberto\4º Curso\Segundo Cuatrimestre\TFG\Saluhud\documentation\SCRUM Planification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaulWorkStation\Documents\TFG\Saluhud\documentation\SCRUM Planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB850C1-3EAA-4B6D-B227-6C8C52DBAACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4299C2D6-6820-4028-A3FA-BF2A731A8233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16575" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23366" yWindow="0" windowWidth="23366" windowHeight="18978" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -170,6 +170,12 @@
   <si>
     <t>Se deben modelar las clases necesarias para el correcto uso de los datos relacionados con las recetas, su visualización y uso.</t>
   </si>
+  <si>
+    <t>Realizar el proceso de bootstrap para Hibernate y asi poder conectarse de forma correcta a la base de datos</t>
+  </si>
+  <si>
+    <t>Configurar C3P0 para soportar conexiones en un entorno de ejecución real</t>
+  </si>
 </sst>
 </file>
 
@@ -277,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -316,9 +322,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -605,22 +608,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G2140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.125" customWidth="1"/>
+    <col min="2" max="2" width="35.875" customWidth="1"/>
+    <col min="3" max="3" width="25.125" customWidth="1"/>
+    <col min="4" max="4" width="20.625" customWidth="1"/>
     <col min="5" max="5" width="57" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="25.375" customWidth="1"/>
+    <col min="7" max="7" width="25.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="14.95" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
@@ -636,7 +639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30.1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
@@ -667,7 +670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>1000</v>
       </c>
@@ -685,7 +688,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>1001</v>
       </c>
@@ -702,7 +705,7 @@
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>1002</v>
       </c>
@@ -711,11 +714,13 @@
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="17"/>
+      <c r="E12" s="13" t="s">
+        <v>44</v>
+      </c>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>1003</v>
       </c>
@@ -724,11 +729,13 @@
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="17"/>
+      <c r="E13" s="13" t="s">
+        <v>45</v>
+      </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>1004</v>
       </c>
@@ -743,7 +750,7 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>1005</v>
       </c>
@@ -758,7 +765,7 @@
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>1006</v>
       </c>
@@ -773,7 +780,7 @@
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>1007</v>
       </c>
@@ -788,7 +795,7 @@
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>1008</v>
       </c>
@@ -803,7 +810,7 @@
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
     </row>
-    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>1009</v>
       </c>
@@ -818,7 +825,7 @@
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
     </row>
-    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>1010</v>
       </c>
@@ -833,7 +840,7 @@
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
     </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>1011</v>
       </c>
@@ -848,7 +855,7 @@
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
     </row>
-    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>1012</v>
       </c>
@@ -863,7 +870,7 @@
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>1013</v>
       </c>
@@ -878,7 +885,7 @@
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -887,7 +894,7 @@
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -896,7 +903,7 @@
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -905,7 +912,7 @@
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -914,7 +921,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -923,7 +930,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -932,7 +939,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -941,7 +948,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -950,11 +957,11 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
         <v>2000</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="17" t="s">
         <v>28</v>
       </c>
       <c r="C32" s="4"/>
@@ -963,11 +970,11 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>2001</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="17" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="4"/>
@@ -976,11 +983,11 @@
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>2002</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="17" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="4"/>
@@ -989,11 +996,11 @@
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>2003</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C35" s="4"/>
@@ -1002,11 +1009,11 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A36" s="16">
         <v>2004</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="17" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="4"/>
@@ -19965,12 +19972,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.75" customWidth="1"/>
+    <col min="2" max="2" width="19.875" customWidth="1"/>
+    <col min="3" max="3" width="20.75" customWidth="1"/>
+    <col min="4" max="4" width="22.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>